<commit_message>
Bolt thrower and Gil-galad fix
</commit_message>
<xml_diff>
--- a/src/data/mesbg_data.xlsx
+++ b/src/data/mesbg_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alex_\Downloads\mesbg-list-builder\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B01ED80B-5A4B-407B-93E7-B0DB76D1D614}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB8A3282-1533-4099-AD8C-FEEF904D17C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="3" xr2:uid="{41642CF3-1564-4507-B9B3-31F38315AF34}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="4" xr2:uid="{41642CF3-1564-4507-B9B3-31F38315AF34}"/>
   </bookViews>
   <sheets>
     <sheet name="models" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14769" uniqueCount="3849">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14773" uniqueCount="3851">
   <si>
     <t>faction</t>
   </si>
@@ -11740,6 +11740,12 @@
   </si>
   <si>
     <t>Aragorn, Strider must be included for the Historical alliance level between The Dead of Dunharrow and The Rangers</t>
+  </si>
+  <si>
+    <t>["[rivendell] elladan_&amp;_elrohir", "[rivendell] lindir", "[rivendell] arwen", "[rivendell] bilbo_baggins"]</t>
+  </si>
+  <si>
+    <t>If Gil-Galad is included in the same force as either Arwen, Lindir, Elladan &amp; Elrohir or Bilbo Baggins, you automatically become Impossible Allies with all armies, and lose your army bonus.</t>
   </si>
 </sst>
 </file>
@@ -12298,7 +12304,7 @@
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A227" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A227" sqref="A227:A536"/>
+      <selection pane="bottomLeft" activeCell="A351" sqref="A351:A361"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -20906,7 +20912,7 @@
         <v>3751</v>
       </c>
     </row>
-    <row r="227" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A227" s="5" t="s">
         <v>1013</v>
       </c>
@@ -25618,7 +25624,7 @@
         <v>842</v>
       </c>
     </row>
-    <row r="351" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="351" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A351" s="5" t="s">
         <v>1057</v>
       </c>
@@ -25656,7 +25662,7 @@
         <v>3747</v>
       </c>
     </row>
-    <row r="352" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="352" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A352" s="5" t="s">
         <v>1058</v>
       </c>
@@ -25694,7 +25700,7 @@
         <v>3771</v>
       </c>
     </row>
-    <row r="353" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="353" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A353" s="5" t="s">
         <v>1059</v>
       </c>
@@ -25732,7 +25738,7 @@
         <v>3797</v>
       </c>
     </row>
-    <row r="354" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="354" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A354" s="5" t="s">
         <v>1060</v>
       </c>
@@ -25770,7 +25776,7 @@
         <v>3751</v>
       </c>
     </row>
-    <row r="355" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="355" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A355" s="5" t="s">
         <v>1061</v>
       </c>
@@ -25808,7 +25814,7 @@
         <v>3797</v>
       </c>
     </row>
-    <row r="356" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="356" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A356" s="5" t="s">
         <v>1062</v>
       </c>
@@ -25846,7 +25852,7 @@
         <v>3758</v>
       </c>
     </row>
-    <row r="357" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="357" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A357" s="5" t="s">
         <v>1063</v>
       </c>
@@ -25884,7 +25890,7 @@
         <v>3797</v>
       </c>
     </row>
-    <row r="358" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="358" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A358" s="5" t="s">
         <v>1064</v>
       </c>
@@ -25922,7 +25928,7 @@
         <v>3772</v>
       </c>
     </row>
-    <row r="359" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="359" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A359" s="5" t="s">
         <v>1065</v>
       </c>
@@ -25960,7 +25966,7 @@
         <v>3788</v>
       </c>
     </row>
-    <row r="360" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="360" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A360" s="5" t="s">
         <v>1066</v>
       </c>
@@ -25998,7 +26004,7 @@
         <v>3772</v>
       </c>
     </row>
-    <row r="361" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="361" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A361" s="5" t="s">
         <v>1570</v>
       </c>
@@ -26036,7 +26042,7 @@
         <v>3802</v>
       </c>
     </row>
-    <row r="362" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="362" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A362" s="5" t="s">
         <v>1067</v>
       </c>
@@ -26074,7 +26080,7 @@
         <v>3758</v>
       </c>
     </row>
-    <row r="363" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="363" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A363" s="5" t="s">
         <v>1966</v>
       </c>
@@ -26112,7 +26118,7 @@
         <v>842</v>
       </c>
     </row>
-    <row r="364" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="364" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A364" s="5" t="s">
         <v>1965</v>
       </c>
@@ -26150,7 +26156,7 @@
         <v>842</v>
       </c>
     </row>
-    <row r="365" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="365" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A365" s="5" t="s">
         <v>1967</v>
       </c>
@@ -29570,7 +29576,7 @@
         <v>3786</v>
       </c>
     </row>
-    <row r="455" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="455" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A455" s="5" t="s">
         <v>1096</v>
       </c>
@@ -32648,7 +32654,7 @@
         <v>3763</v>
       </c>
     </row>
-    <row r="536" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="536" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A536" s="5" t="s">
         <v>1522</v>
       </c>
@@ -46330,15 +46336,9 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:L895" xr:uid="{7E32720F-3682-46D9-B418-543447137BE7}">
-    <filterColumn colId="1">
+    <filterColumn colId="2">
       <filters>
-        <filter val="Good Army"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="4">
-      <filters>
-        <filter val="Aragorn, King Elessar"/>
-        <filter val="Aragorn, Strider"/>
+        <filter val="Rivendell"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -46357,9 +46357,9 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:G1649"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A289" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C335" sqref="C335"/>
+    <sheetView topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A485" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D486" sqref="D486"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -52559,7 +52559,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="289" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="289" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A289" s="9" t="s">
         <v>600</v>
       </c>
@@ -52580,7 +52580,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="290" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="290" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A290" s="9" t="s">
         <v>602</v>
       </c>
@@ -52601,7 +52601,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="291" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="291" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A291" s="9" t="s">
         <v>603</v>
       </c>
@@ -52622,7 +52622,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="292" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="292" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A292" s="9" t="s">
         <v>604</v>
       </c>
@@ -52643,7 +52643,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="293" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="293" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A293" s="9" t="s">
         <v>605</v>
       </c>
@@ -52664,7 +52664,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="294" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="294" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A294" s="9" t="s">
         <v>606</v>
       </c>
@@ -53539,7 +53539,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="335" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="335" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A335" s="9" t="s">
         <v>653</v>
       </c>
@@ -53560,7 +53560,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="336" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="336" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A336" s="9" t="s">
         <v>654</v>
       </c>
@@ -53581,7 +53581,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="337" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="337" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A337" s="9" t="s">
         <v>655</v>
       </c>
@@ -53602,7 +53602,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="338" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="338" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A338" s="9" t="s">
         <v>656</v>
       </c>
@@ -53623,7 +53623,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="339" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="339" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A339" s="9" t="s">
         <v>657</v>
       </c>
@@ -53644,7 +53644,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="340" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="340" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A340" s="9" t="s">
         <v>658</v>
       </c>
@@ -53665,7 +53665,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="341" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="341" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A341" s="9" t="s">
         <v>659</v>
       </c>
@@ -53686,7 +53686,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="342" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="342" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A342" s="9" t="s">
         <v>660</v>
       </c>
@@ -53709,7 +53709,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="343" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="343" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A343" s="9" t="s">
         <v>661</v>
       </c>
@@ -53730,7 +53730,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="344" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="344" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A344" s="9" t="s">
         <v>662</v>
       </c>
@@ -53751,7 +53751,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="345" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="345" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A345" s="9" t="s">
         <v>663</v>
       </c>
@@ -53772,7 +53772,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="346" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="346" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A346" s="9" t="s">
         <v>664</v>
       </c>
@@ -53793,7 +53793,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="347" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="347" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A347" s="9" t="s">
         <v>665</v>
       </c>
@@ -56755,7 +56755,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="485" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="485" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A485" s="9" t="s">
         <v>818</v>
       </c>
@@ -56766,7 +56766,7 @@
         <v>449</v>
       </c>
       <c r="D485" s="6">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="E485" s="6" t="s">
         <v>3838</v>
@@ -56778,7 +56778,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="486" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="486" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A486" s="9" t="s">
         <v>819</v>
       </c>
@@ -56799,7 +56799,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="487" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="487" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A487" s="9" t="s">
         <v>820</v>
       </c>
@@ -72126,7 +72126,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1196" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1196" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A1196" s="9" t="s">
         <v>2532</v>
       </c>
@@ -72147,7 +72147,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1197" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1197" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A1197" s="9" t="s">
         <v>2533</v>
       </c>
@@ -72170,7 +72170,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1198" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1198" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A1198" s="9" t="s">
         <v>2534</v>
       </c>
@@ -72191,7 +72191,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1199" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1199" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A1199" s="9" t="s">
         <v>2535</v>
       </c>
@@ -72212,7 +72212,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1200" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1200" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A1200" s="9" t="s">
         <v>2536</v>
       </c>
@@ -72233,7 +72233,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1201" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1201" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A1201" s="9" t="s">
         <v>2537</v>
       </c>
@@ -72254,7 +72254,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1202" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1202" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A1202" s="9" t="s">
         <v>2538</v>
       </c>
@@ -81648,10 +81648,7 @@
   <autoFilter ref="A1:G1649" xr:uid="{6BD621D9-338F-4B24-B8C0-543A62D24772}">
     <filterColumn colId="1">
       <filters>
-        <filter val="[far_harad] war_mumak_of_far_harad"/>
-        <filter val="[grand_army_of_the_south] war_mumak_of_grand_army_of_the_south"/>
-        <filter val="[grand_army_of_the_south] war_mumak_of_harad"/>
-        <filter val="[the_serpent_horde] war_mumak_of_harad"/>
+        <filter val="[minas_tirith] avenger_bolt_thrower"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -83065,7 +83062,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59CB009E-54DD-49E7-AF48-1368091BE4E1}">
   <dimension ref="A1:E618"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A389" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B399" sqref="B399"/>
     </sheetView>
@@ -92199,10 +92196,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{041E0963-E2E9-41B5-B435-BC1A1C291BC2}">
-  <dimension ref="A1:D90"/>
+  <dimension ref="A1:D91"/>
   <sheetViews>
-    <sheetView topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="C92" sqref="C92"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="13" x14ac:dyDescent="0.35"/>
@@ -92424,144 +92421,144 @@
         <v>2715</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" ht="26" x14ac:dyDescent="0.35">
       <c r="A16" s="12" t="s">
-        <v>944</v>
+        <v>1065</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>1592</v>
+        <v>1549</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>1613</v>
+        <v>3849</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>1593</v>
+        <v>3850</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="12" t="s">
-        <v>1594</v>
+        <v>944</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>3133</v>
+        <v>1592</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>1595</v>
+        <v>1613</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>1596</v>
+        <v>1593</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="12" t="s">
-        <v>1599</v>
+        <v>1594</v>
       </c>
       <c r="B18" s="12" t="s">
         <v>3133</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>1597</v>
+        <v>1595</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>1598</v>
+        <v>1596</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="12" t="s">
-        <v>839</v>
+        <v>1599</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>1592</v>
+        <v>3133</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>1631</v>
+        <v>1597</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>1632</v>
+        <v>1598</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="12" t="s">
-        <v>1636</v>
+        <v>839</v>
       </c>
       <c r="B20" s="12" t="s">
         <v>1592</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>1667</v>
+        <v>1631</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>1668</v>
+        <v>1632</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="12" t="s">
-        <v>942</v>
+        <v>1636</v>
       </c>
       <c r="B21" s="12" t="s">
         <v>1592</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>1710</v>
+        <v>1667</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>1709</v>
+        <v>1668</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="12" t="s">
-        <v>868</v>
+        <v>942</v>
       </c>
       <c r="B22" s="12" t="s">
         <v>1592</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>1751</v>
+        <v>1710</v>
       </c>
       <c r="D22" s="11" t="s">
-        <v>1668</v>
+        <v>1709</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="12" t="s">
-        <v>867</v>
+        <v>868</v>
       </c>
       <c r="B23" s="12" t="s">
         <v>1592</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>1780</v>
+        <v>1751</v>
       </c>
       <c r="D23" s="11" t="s">
-        <v>1779</v>
+        <v>1668</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="12" t="s">
-        <v>840</v>
+        <v>867</v>
       </c>
       <c r="B24" s="12" t="s">
         <v>1592</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>1801</v>
+        <v>1780</v>
       </c>
       <c r="D24" s="11" t="s">
-        <v>1800</v>
+        <v>1779</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="12" t="s">
-        <v>881</v>
+        <v>840</v>
       </c>
       <c r="B25" s="12" t="s">
         <v>1592</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>1835</v>
+        <v>1801</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>1668</v>
+        <v>1800</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
@@ -92572,10 +92569,10 @@
         <v>1592</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>1836</v>
+        <v>1835</v>
       </c>
       <c r="D26" s="11" t="s">
-        <v>1837</v>
+        <v>1668</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
@@ -92586,52 +92583,52 @@
         <v>1592</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>1834</v>
+        <v>1836</v>
       </c>
       <c r="D27" s="11" t="s">
-        <v>1838</v>
+        <v>1837</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" s="12" t="s">
-        <v>891</v>
+        <v>881</v>
       </c>
       <c r="B28" s="12" t="s">
         <v>1592</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>1861</v>
+        <v>1834</v>
       </c>
       <c r="D28" s="11" t="s">
-        <v>1862</v>
+        <v>1838</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" s="12" t="s">
-        <v>866</v>
+        <v>891</v>
       </c>
       <c r="B29" s="12" t="s">
         <v>1592</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>1884</v>
+        <v>1861</v>
       </c>
       <c r="D29" s="11" t="s">
-        <v>1632</v>
+        <v>1862</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" s="12" t="s">
-        <v>957</v>
+        <v>866</v>
       </c>
       <c r="B30" s="12" t="s">
         <v>1592</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>1920</v>
+        <v>1884</v>
       </c>
       <c r="D30" s="11" t="s">
-        <v>2091</v>
+        <v>1632</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
@@ -92642,41 +92639,41 @@
         <v>1592</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>1919</v>
+        <v>1920</v>
       </c>
       <c r="D31" s="11" t="s">
-        <v>2090</v>
+        <v>2091</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" s="12" t="s">
-        <v>854</v>
+        <v>957</v>
       </c>
       <c r="B32" s="12" t="s">
         <v>1592</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>2089</v>
+        <v>1919</v>
       </c>
       <c r="D32" s="11" t="s">
-        <v>2092</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="26" x14ac:dyDescent="0.35">
+        <v>2090</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" s="12" t="s">
-        <v>945</v>
+        <v>854</v>
       </c>
       <c r="B33" s="12" t="s">
         <v>1592</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>2153</v>
+        <v>2089</v>
       </c>
       <c r="D33" s="11" t="s">
-        <v>2154</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="39" x14ac:dyDescent="0.35">
+        <v>2092</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="26" x14ac:dyDescent="0.35">
       <c r="A34" s="12" t="s">
         <v>945</v>
       </c>
@@ -92684,80 +92681,80 @@
         <v>1592</v>
       </c>
       <c r="C34" s="11" t="s">
-        <v>2155</v>
+        <v>2153</v>
       </c>
       <c r="D34" s="11" t="s">
-        <v>2156</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+        <v>2154</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="39" x14ac:dyDescent="0.35">
       <c r="A35" s="12" t="s">
-        <v>855</v>
+        <v>945</v>
       </c>
       <c r="B35" s="12" t="s">
         <v>1592</v>
       </c>
       <c r="C35" s="11" t="s">
-        <v>2702</v>
+        <v>2155</v>
       </c>
       <c r="D35" s="11" t="s">
-        <v>2703</v>
+        <v>2156</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" s="12" t="s">
-        <v>849</v>
+        <v>855</v>
       </c>
       <c r="B36" s="12" t="s">
         <v>1592</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>2192</v>
+        <v>2702</v>
       </c>
       <c r="D36" s="11" t="s">
-        <v>2193</v>
+        <v>2703</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" s="12" t="s">
-        <v>916</v>
+        <v>849</v>
       </c>
       <c r="B37" s="12" t="s">
         <v>1592</v>
       </c>
       <c r="C37" s="11" t="s">
-        <v>2217</v>
+        <v>2192</v>
       </c>
       <c r="D37" s="11" t="s">
-        <v>2218</v>
+        <v>2193</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" s="12" t="s">
-        <v>911</v>
+        <v>916</v>
       </c>
       <c r="B38" s="12" t="s">
         <v>1592</v>
       </c>
       <c r="C38" s="11" t="s">
-        <v>2225</v>
+        <v>2217</v>
       </c>
       <c r="D38" s="11" t="s">
-        <v>2226</v>
+        <v>2218</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" s="12" t="s">
-        <v>919</v>
+        <v>911</v>
       </c>
       <c r="B39" s="12" t="s">
         <v>1592</v>
       </c>
       <c r="C39" s="11" t="s">
-        <v>2262</v>
+        <v>2225</v>
       </c>
       <c r="D39" s="11" t="s">
-        <v>2260</v>
+        <v>2226</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.35">
@@ -92768,94 +92765,94 @@
         <v>1592</v>
       </c>
       <c r="C40" s="11" t="s">
-        <v>2263</v>
+        <v>2262</v>
       </c>
       <c r="D40" s="11" t="s">
-        <v>2261</v>
+        <v>2260</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" s="12" t="s">
-        <v>850</v>
+        <v>919</v>
       </c>
       <c r="B41" s="12" t="s">
         <v>1592</v>
       </c>
       <c r="C41" s="11" t="s">
-        <v>2587</v>
+        <v>2263</v>
       </c>
       <c r="D41" s="11" t="s">
-        <v>2588</v>
+        <v>2261</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" s="12" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="B42" s="12" t="s">
         <v>1592</v>
       </c>
       <c r="C42" s="11" t="s">
-        <v>2614</v>
+        <v>2587</v>
       </c>
       <c r="D42" s="11" t="s">
-        <v>2615</v>
+        <v>2588</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" s="12" t="s">
-        <v>2632</v>
+        <v>851</v>
       </c>
       <c r="B43" s="12" t="s">
         <v>1592</v>
       </c>
       <c r="C43" s="11" t="s">
-        <v>3745</v>
+        <v>2614</v>
       </c>
       <c r="D43" s="11" t="s">
-        <v>3744</v>
+        <v>2615</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" s="12" t="s">
-        <v>887</v>
+        <v>2632</v>
       </c>
       <c r="B44" s="12" t="s">
         <v>1592</v>
       </c>
       <c r="C44" s="11" t="s">
+        <v>3745</v>
+      </c>
+      <c r="D44" s="11" t="s">
+        <v>3744</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A45" s="12" t="s">
+        <v>887</v>
+      </c>
+      <c r="B45" s="12" t="s">
+        <v>1592</v>
+      </c>
+      <c r="C45" s="11" t="s">
         <v>2666</v>
       </c>
-      <c r="D44" s="11" t="s">
+      <c r="D45" s="11" t="s">
         <v>2667</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="65" x14ac:dyDescent="0.35">
-      <c r="A45" s="12" t="s">
+    <row r="46" spans="1:4" ht="65" x14ac:dyDescent="0.35">
+      <c r="A46" s="12" t="s">
         <v>2669</v>
       </c>
-      <c r="B45" s="12" t="s">
+      <c r="B46" s="12" t="s">
         <v>3133</v>
       </c>
-      <c r="C45" s="11" t="s">
+      <c r="C46" s="11" t="s">
         <v>2688</v>
       </c>
-      <c r="D45" s="11" t="s">
+      <c r="D46" s="11" t="s">
         <v>2689</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A46" s="12" t="s">
-        <v>944</v>
-      </c>
-      <c r="B46" s="12" t="s">
-        <v>1592</v>
-      </c>
-      <c r="C46" s="11" t="s">
-        <v>2711</v>
-      </c>
-      <c r="D46" s="11" t="s">
-        <v>2708</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.35">
@@ -92866,10 +92863,10 @@
         <v>1592</v>
       </c>
       <c r="C47" s="11" t="s">
-        <v>2712</v>
+        <v>2711</v>
       </c>
       <c r="D47" s="11" t="s">
-        <v>2709</v>
+        <v>2708</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.35">
@@ -92880,85 +92877,85 @@
         <v>1592</v>
       </c>
       <c r="C48" s="11" t="s">
+        <v>2712</v>
+      </c>
+      <c r="D48" s="11" t="s">
+        <v>2709</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A49" s="12" t="s">
+        <v>944</v>
+      </c>
+      <c r="B49" s="12" t="s">
+        <v>1592</v>
+      </c>
+      <c r="C49" s="11" t="s">
         <v>2713</v>
       </c>
-      <c r="D48" s="11" t="s">
+      <c r="D49" s="11" t="s">
         <v>2710</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="26" x14ac:dyDescent="0.35">
-      <c r="A49" s="12" t="s">
+    <row r="50" spans="1:4" ht="26" x14ac:dyDescent="0.35">
+      <c r="A50" s="12" t="s">
         <v>2733</v>
-      </c>
-      <c r="B49" s="12" t="s">
-        <v>1549</v>
-      </c>
-      <c r="C49" s="11" t="s">
-        <v>2732</v>
-      </c>
-      <c r="D49" s="11" t="s">
-        <v>2734</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" ht="52" x14ac:dyDescent="0.35">
-      <c r="A50" s="12" t="s">
-        <v>2992</v>
       </c>
       <c r="B50" s="12" t="s">
         <v>1549</v>
       </c>
       <c r="C50" s="11" t="s">
+        <v>2732</v>
+      </c>
+      <c r="D50" s="11" t="s">
+        <v>2734</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="52" x14ac:dyDescent="0.35">
+      <c r="A51" s="12" t="s">
+        <v>2992</v>
+      </c>
+      <c r="B51" s="12" t="s">
+        <v>1549</v>
+      </c>
+      <c r="C51" s="11" t="s">
         <v>2993</v>
       </c>
-      <c r="D50" s="11" t="s">
+      <c r="D51" s="11" t="s">
         <v>2971</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" ht="26" x14ac:dyDescent="0.35">
-      <c r="A51" s="12" t="s">
-        <v>3103</v>
-      </c>
-      <c r="B51" s="12" t="s">
-        <v>3134</v>
-      </c>
-      <c r="C51" s="11" t="s">
-        <v>3122</v>
-      </c>
-      <c r="D51" s="11" t="s">
-        <v>3136</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="26" x14ac:dyDescent="0.35">
       <c r="A52" s="12" t="s">
+        <v>3103</v>
+      </c>
+      <c r="B52" s="12" t="s">
+        <v>3134</v>
+      </c>
+      <c r="C52" s="11" t="s">
+        <v>3122</v>
+      </c>
+      <c r="D52" s="11" t="s">
+        <v>3136</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="26" x14ac:dyDescent="0.35">
+      <c r="A53" s="12" t="s">
         <v>3120</v>
-      </c>
-      <c r="B52" s="12" t="s">
-        <v>3133</v>
-      </c>
-      <c r="C52" s="11" t="s">
-        <v>3135</v>
-      </c>
-      <c r="D52" s="11" t="s">
-        <v>3137</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A53" s="12" t="s">
-        <v>3260</v>
       </c>
       <c r="B53" s="12" t="s">
         <v>3133</v>
       </c>
-      <c r="C53" s="13" t="s">
-        <v>3261</v>
+      <c r="C53" s="11" t="s">
+        <v>3135</v>
       </c>
       <c r="D53" s="11" t="s">
-        <v>3687</v>
+        <v>3137</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" s="12" t="s">
-        <v>3262</v>
+        <v>3260</v>
       </c>
       <c r="B54" s="12" t="s">
         <v>3133</v>
@@ -92967,12 +92964,12 @@
         <v>3261</v>
       </c>
       <c r="D54" s="11" t="s">
-        <v>3688</v>
+        <v>3687</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" s="12" t="s">
-        <v>3263</v>
+        <v>3262</v>
       </c>
       <c r="B55" s="12" t="s">
         <v>3133</v>
@@ -92981,12 +92978,12 @@
         <v>3261</v>
       </c>
       <c r="D55" s="11" t="s">
-        <v>3689</v>
+        <v>3688</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" s="12" t="s">
-        <v>3694</v>
+        <v>3263</v>
       </c>
       <c r="B56" s="12" t="s">
         <v>3133</v>
@@ -92995,26 +92992,26 @@
         <v>3261</v>
       </c>
       <c r="D56" s="11" t="s">
-        <v>3690</v>
+        <v>3689</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" s="12" t="s">
-        <v>3269</v>
+        <v>3694</v>
       </c>
       <c r="B57" s="12" t="s">
         <v>3133</v>
       </c>
-      <c r="C57" s="11" t="s">
-        <v>3275</v>
+      <c r="C57" s="13" t="s">
+        <v>3261</v>
       </c>
       <c r="D57" s="11" t="s">
-        <v>3273</v>
+        <v>3690</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" s="12" t="s">
-        <v>3270</v>
+        <v>3269</v>
       </c>
       <c r="B58" s="12" t="s">
         <v>3133</v>
@@ -93023,12 +93020,12 @@
         <v>3275</v>
       </c>
       <c r="D58" s="11" t="s">
-        <v>3274</v>
+        <v>3273</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" s="12" t="s">
-        <v>3271</v>
+        <v>3270</v>
       </c>
       <c r="B59" s="12" t="s">
         <v>3133</v>
@@ -93037,12 +93034,12 @@
         <v>3275</v>
       </c>
       <c r="D59" s="11" t="s">
-        <v>3276</v>
+        <v>3274</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" s="12" t="s">
-        <v>3272</v>
+        <v>3271</v>
       </c>
       <c r="B60" s="12" t="s">
         <v>3133</v>
@@ -93051,26 +93048,26 @@
         <v>3275</v>
       </c>
       <c r="D60" s="11" t="s">
+        <v>3276</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A61" s="12" t="s">
+        <v>3272</v>
+      </c>
+      <c r="B61" s="12" t="s">
+        <v>3133</v>
+      </c>
+      <c r="C61" s="11" t="s">
+        <v>3275</v>
+      </c>
+      <c r="D61" s="11" t="s">
         <v>3277</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" ht="26" x14ac:dyDescent="0.35">
-      <c r="A61" s="12" t="s">
-        <v>3269</v>
-      </c>
-      <c r="B61" s="12" t="s">
-        <v>3278</v>
-      </c>
-      <c r="C61" s="11" t="s">
-        <v>3279</v>
-      </c>
-      <c r="D61" s="11" t="s">
-        <v>3280</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="26" x14ac:dyDescent="0.35">
       <c r="A62" s="12" t="s">
-        <v>3270</v>
+        <v>3269</v>
       </c>
       <c r="B62" s="12" t="s">
         <v>3278</v>
@@ -93084,7 +93081,7 @@
     </row>
     <row r="63" spans="1:4" ht="26" x14ac:dyDescent="0.35">
       <c r="A63" s="12" t="s">
-        <v>3271</v>
+        <v>3270</v>
       </c>
       <c r="B63" s="12" t="s">
         <v>3278</v>
@@ -93098,7 +93095,7 @@
     </row>
     <row r="64" spans="1:4" ht="26" x14ac:dyDescent="0.35">
       <c r="A64" s="12" t="s">
-        <v>3272</v>
+        <v>3271</v>
       </c>
       <c r="B64" s="12" t="s">
         <v>3278</v>
@@ -93112,7 +93109,7 @@
     </row>
     <row r="65" spans="1:4" ht="26" x14ac:dyDescent="0.35">
       <c r="A65" s="12" t="s">
-        <v>1528</v>
+        <v>3272</v>
       </c>
       <c r="B65" s="12" t="s">
         <v>3278</v>
@@ -93121,12 +93118,12 @@
         <v>3279</v>
       </c>
       <c r="D65" s="11" t="s">
-        <v>3281</v>
+        <v>3280</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="26" x14ac:dyDescent="0.35">
       <c r="A66" s="12" t="s">
-        <v>1532</v>
+        <v>1528</v>
       </c>
       <c r="B66" s="12" t="s">
         <v>3278</v>
@@ -93135,12 +93132,12 @@
         <v>3279</v>
       </c>
       <c r="D66" s="11" t="s">
-        <v>3282</v>
+        <v>3281</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="26" x14ac:dyDescent="0.35">
       <c r="A67" s="12" t="s">
-        <v>1527</v>
+        <v>1532</v>
       </c>
       <c r="B67" s="12" t="s">
         <v>3278</v>
@@ -93149,49 +93146,49 @@
         <v>3279</v>
       </c>
       <c r="D67" s="11" t="s">
+        <v>3282</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" ht="26" x14ac:dyDescent="0.35">
+      <c r="A68" s="12" t="s">
+        <v>1527</v>
+      </c>
+      <c r="B68" s="12" t="s">
+        <v>3278</v>
+      </c>
+      <c r="C68" s="11" t="s">
+        <v>3279</v>
+      </c>
+      <c r="D68" s="11" t="s">
         <v>3283</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" ht="26" x14ac:dyDescent="0.35">
-      <c r="A68" s="24" t="s">
-        <v>3311</v>
-      </c>
-      <c r="B68" s="12" t="s">
-        <v>3133</v>
-      </c>
-      <c r="C68" s="11" t="s">
-        <v>3312</v>
-      </c>
-      <c r="D68" s="11" t="s">
-        <v>3313</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="26" x14ac:dyDescent="0.35">
       <c r="A69" s="24" t="s">
-        <v>3333</v>
+        <v>3311</v>
       </c>
       <c r="B69" s="12" t="s">
         <v>3133</v>
       </c>
       <c r="C69" s="11" t="s">
+        <v>3312</v>
+      </c>
+      <c r="D69" s="11" t="s">
+        <v>3313</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="26" x14ac:dyDescent="0.35">
+      <c r="A70" s="24" t="s">
+        <v>3333</v>
+      </c>
+      <c r="B70" s="12" t="s">
+        <v>3133</v>
+      </c>
+      <c r="C70" s="11" t="s">
         <v>3335</v>
       </c>
-      <c r="D69" s="11" t="s">
+      <c r="D70" s="11" t="s">
         <v>3336</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A70" s="6" t="s">
-        <v>928</v>
-      </c>
-      <c r="B70" s="12" t="s">
-        <v>1592</v>
-      </c>
-      <c r="C70" s="11" t="s">
-        <v>3386</v>
-      </c>
-      <c r="D70" s="11" t="s">
-        <v>3389</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
@@ -93202,10 +93199,10 @@
         <v>1592</v>
       </c>
       <c r="C71" s="11" t="s">
-        <v>3387</v>
+        <v>3386</v>
       </c>
       <c r="D71" s="11" t="s">
-        <v>3398</v>
+        <v>3389</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
@@ -93216,55 +93213,55 @@
         <v>1592</v>
       </c>
       <c r="C72" s="11" t="s">
-        <v>3388</v>
+        <v>3387</v>
       </c>
       <c r="D72" s="11" t="s">
-        <v>3397</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" ht="26" x14ac:dyDescent="0.35">
-      <c r="A73" s="12" t="s">
-        <v>929</v>
+        <v>3398</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A73" s="6" t="s">
+        <v>928</v>
       </c>
       <c r="B73" s="12" t="s">
         <v>1592</v>
       </c>
       <c r="C73" s="11" t="s">
-        <v>3395</v>
+        <v>3388</v>
       </c>
       <c r="D73" s="11" t="s">
-        <v>3396</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
+        <v>3397</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" ht="26" x14ac:dyDescent="0.35">
       <c r="A74" s="12" t="s">
-        <v>885</v>
+        <v>929</v>
       </c>
       <c r="B74" s="12" t="s">
         <v>1592</v>
       </c>
       <c r="C74" s="11" t="s">
-        <v>3425</v>
+        <v>3395</v>
       </c>
       <c r="D74" s="11" t="s">
-        <v>3426</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" ht="104" x14ac:dyDescent="0.35">
+        <v>3396</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75" s="12" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="B75" s="12" t="s">
         <v>1592</v>
       </c>
       <c r="C75" s="11" t="s">
-        <v>3551</v>
+        <v>3425</v>
       </c>
       <c r="D75" s="11" t="s">
-        <v>3496</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" ht="26" x14ac:dyDescent="0.35">
+        <v>3426</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" ht="104" x14ac:dyDescent="0.35">
       <c r="A76" s="12" t="s">
         <v>886</v>
       </c>
@@ -93272,66 +93269,66 @@
         <v>1592</v>
       </c>
       <c r="C76" s="11" t="s">
-        <v>3552</v>
+        <v>3551</v>
       </c>
       <c r="D76" s="11" t="s">
-        <v>3495</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
+        <v>3496</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" ht="26" x14ac:dyDescent="0.35">
       <c r="A77" s="12" t="s">
-        <v>953</v>
+        <v>886</v>
       </c>
       <c r="B77" s="12" t="s">
         <v>1592</v>
       </c>
       <c r="C77" s="11" t="s">
-        <v>3493</v>
+        <v>3552</v>
       </c>
       <c r="D77" s="11" t="s">
-        <v>3494</v>
+        <v>3495</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A78" s="12" t="s">
-        <v>935</v>
+        <v>953</v>
       </c>
       <c r="B78" s="12" t="s">
         <v>1592</v>
       </c>
       <c r="C78" s="11" t="s">
-        <v>3513</v>
+        <v>3493</v>
       </c>
       <c r="D78" s="11" t="s">
-        <v>3514</v>
+        <v>3494</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A79" s="12" t="s">
-        <v>950</v>
+        <v>935</v>
       </c>
       <c r="B79" s="12" t="s">
         <v>1592</v>
       </c>
       <c r="C79" s="11" t="s">
-        <v>3548</v>
+        <v>3513</v>
       </c>
       <c r="D79" s="11" t="s">
-        <v>3549</v>
+        <v>3514</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A80" s="12" t="s">
-        <v>939</v>
+        <v>950</v>
       </c>
       <c r="B80" s="12" t="s">
         <v>1592</v>
       </c>
       <c r="C80" s="11" t="s">
-        <v>3596</v>
+        <v>3548</v>
       </c>
       <c r="D80" s="11" t="s">
-        <v>3597</v>
+        <v>3549</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.35">
@@ -93342,24 +93339,24 @@
         <v>1592</v>
       </c>
       <c r="C81" s="11" t="s">
-        <v>3599</v>
+        <v>3596</v>
       </c>
       <c r="D81" s="11" t="s">
-        <v>3598</v>
+        <v>3597</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A82" s="12" t="s">
-        <v>242</v>
+        <v>939</v>
       </c>
       <c r="B82" s="12" t="s">
         <v>1592</v>
       </c>
       <c r="C82" s="11" t="s">
-        <v>3600</v>
+        <v>3599</v>
       </c>
       <c r="D82" s="11" t="s">
-        <v>3601</v>
+        <v>3598</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.35">
@@ -93370,94 +93367,94 @@
         <v>1592</v>
       </c>
       <c r="C83" s="11" t="s">
-        <v>3603</v>
+        <v>3600</v>
       </c>
       <c r="D83" s="11" t="s">
-        <v>3602</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A84" s="6" t="s">
-        <v>241</v>
+        <v>3601</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A84" s="12" t="s">
+        <v>242</v>
       </c>
       <c r="B84" s="12" t="s">
         <v>1592</v>
       </c>
       <c r="C84" s="11" t="s">
+        <v>3603</v>
+      </c>
+      <c r="D84" s="11" t="s">
+        <v>3602</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A85" s="6" t="s">
+        <v>241</v>
+      </c>
+      <c r="B85" s="12" t="s">
+        <v>1592</v>
+      </c>
+      <c r="C85" s="11" t="s">
         <v>3605</v>
       </c>
-      <c r="D84" s="11" t="s">
+      <c r="D85" s="11" t="s">
         <v>3606</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" ht="26" x14ac:dyDescent="0.35">
-      <c r="A85" s="12" t="s">
-        <v>3643</v>
-      </c>
-      <c r="B85" s="12" t="s">
-        <v>3672</v>
-      </c>
-      <c r="C85" s="11" t="s">
-        <v>3675</v>
-      </c>
-      <c r="D85" s="11" t="s">
-        <v>3670</v>
       </c>
     </row>
     <row r="86" spans="1:4" ht="26" x14ac:dyDescent="0.35">
       <c r="A86" s="12" t="s">
-        <v>3644</v>
+        <v>3643</v>
       </c>
       <c r="B86" s="12" t="s">
         <v>3672</v>
       </c>
       <c r="C86" s="11" t="s">
-        <v>3674</v>
+        <v>3675</v>
       </c>
       <c r="D86" s="11" t="s">
-        <v>3695</v>
+        <v>3670</v>
       </c>
     </row>
     <row r="87" spans="1:4" ht="26" x14ac:dyDescent="0.35">
       <c r="A87" s="12" t="s">
-        <v>3399</v>
+        <v>3644</v>
       </c>
       <c r="B87" s="12" t="s">
         <v>3672</v>
       </c>
       <c r="C87" s="11" t="s">
-        <v>3676</v>
+        <v>3674</v>
       </c>
       <c r="D87" s="11" t="s">
-        <v>3671</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
+        <v>3695</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" ht="26" x14ac:dyDescent="0.35">
       <c r="A88" s="12" t="s">
-        <v>2910</v>
+        <v>3399</v>
       </c>
       <c r="B88" s="12" t="s">
         <v>3672</v>
       </c>
       <c r="C88" s="11" t="s">
-        <v>3677</v>
+        <v>3676</v>
       </c>
       <c r="D88" s="11" t="s">
-        <v>3673</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" ht="26" x14ac:dyDescent="0.35">
+        <v>3671</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A89" s="12" t="s">
-        <v>239</v>
+        <v>2910</v>
       </c>
       <c r="B89" s="12" t="s">
         <v>3672</v>
       </c>
       <c r="C89" s="11" t="s">
-        <v>3846</v>
+        <v>3677</v>
       </c>
       <c r="D89" s="11" t="s">
-        <v>3847</v>
+        <v>3673</v>
       </c>
     </row>
     <row r="90" spans="1:4" ht="26" x14ac:dyDescent="0.35">
@@ -93468,9 +93465,23 @@
         <v>3672</v>
       </c>
       <c r="C90" s="11" t="s">
+        <v>3846</v>
+      </c>
+      <c r="D90" s="11" t="s">
+        <v>3847</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" ht="26" x14ac:dyDescent="0.35">
+      <c r="A91" s="12" t="s">
+        <v>239</v>
+      </c>
+      <c r="B91" s="12" t="s">
+        <v>3672</v>
+      </c>
+      <c r="C91" s="11" t="s">
         <v>3845</v>
       </c>
-      <c r="D90" s="11" t="s">
+      <c r="D91" s="11" t="s">
         <v>3848</v>
       </c>
     </row>

</xml_diff>

<commit_message>
50% bow limit dependency
</commit_message>
<xml_diff>
--- a/src/data/mesbg_data.xlsx
+++ b/src/data/mesbg_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alex_\Downloads\mesbg-list-builder\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB8A3282-1533-4099-AD8C-FEEF904D17C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD4582AB-594C-4FBC-ADA7-D70510206B0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="4" xr2:uid="{41642CF3-1564-4507-B9B3-31F38315AF34}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="2" xr2:uid="{41642CF3-1564-4507-B9B3-31F38315AF34}"/>
   </bookViews>
   <sheets>
     <sheet name="models" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="warning_rules" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">factions!$A$1:$E$89</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">hero_constraints!$A$1:$E$511</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">models!$A$1:$L$895</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">options!$A$1:$G$1649</definedName>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14773" uniqueCount="3851">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14772" uniqueCount="3851">
   <si>
     <t>faction</t>
   </si>
@@ -81664,10 +81665,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46B3BDA4-C76D-4F2B-A5C7-6A022A2D593F}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:E89"/>
   <sheetViews>
-    <sheetView topLeftCell="A51" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A54" sqref="A54"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B74" sqref="B74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -81696,7 +81698,7 @@
         <v>1547</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="91" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="91" hidden="1" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="s">
         <v>131</v>
       </c>
@@ -81713,7 +81715,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="39" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="39" hidden="1" x14ac:dyDescent="0.35">
       <c r="A3" s="10" t="s">
         <v>95</v>
       </c>
@@ -81730,7 +81732,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="143" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" ht="143" hidden="1" x14ac:dyDescent="0.35">
       <c r="A4" s="10" t="s">
         <v>123</v>
       </c>
@@ -81747,7 +81749,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="130" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" ht="130" hidden="1" x14ac:dyDescent="0.35">
       <c r="A5" s="10" t="s">
         <v>1636</v>
       </c>
@@ -81760,7 +81762,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="78" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" ht="78" hidden="1" x14ac:dyDescent="0.35">
       <c r="A6" s="10" t="s">
         <v>3</v>
       </c>
@@ -81777,7 +81779,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="91" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" ht="91" hidden="1" x14ac:dyDescent="0.35">
       <c r="A7" s="10" t="s">
         <v>834</v>
       </c>
@@ -81794,7 +81796,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="78" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" ht="78" hidden="1" x14ac:dyDescent="0.35">
       <c r="A8" s="10" t="s">
         <v>71</v>
       </c>
@@ -81811,7 +81813,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="39" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" ht="39" hidden="1" x14ac:dyDescent="0.35">
       <c r="A9" s="10" t="s">
         <v>838</v>
       </c>
@@ -81828,7 +81830,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="130" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" ht="130" hidden="1" x14ac:dyDescent="0.35">
       <c r="A10" s="10" t="s">
         <v>839</v>
       </c>
@@ -81841,7 +81843,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="104" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" ht="104" hidden="1" x14ac:dyDescent="0.35">
       <c r="A11" s="10" t="s">
         <v>840</v>
       </c>
@@ -81854,7 +81856,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="39" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" ht="39" hidden="1" x14ac:dyDescent="0.35">
       <c r="A12" s="10" t="s">
         <v>238</v>
       </c>
@@ -81871,7 +81873,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="65" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" ht="65" hidden="1" x14ac:dyDescent="0.35">
       <c r="A13" s="10" t="s">
         <v>844</v>
       </c>
@@ -81888,7 +81890,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="52" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" ht="52" hidden="1" x14ac:dyDescent="0.35">
       <c r="A14" s="10" t="s">
         <v>42</v>
       </c>
@@ -81905,7 +81907,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="195" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" ht="195" hidden="1" x14ac:dyDescent="0.35">
       <c r="A15" s="10" t="s">
         <v>849</v>
       </c>
@@ -81918,7 +81920,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="221" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" ht="221" hidden="1" x14ac:dyDescent="0.35">
       <c r="A16" s="10" t="s">
         <v>850</v>
       </c>
@@ -81931,7 +81933,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="299" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" ht="299" hidden="1" x14ac:dyDescent="0.35">
       <c r="A17" s="10" t="s">
         <v>851</v>
       </c>
@@ -81944,7 +81946,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="78" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" ht="78" hidden="1" x14ac:dyDescent="0.35">
       <c r="A18" s="10" t="s">
         <v>3024</v>
       </c>
@@ -81961,7 +81963,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="52" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" ht="52" hidden="1" x14ac:dyDescent="0.35">
       <c r="A19" s="10" t="s">
         <v>3022</v>
       </c>
@@ -81978,7 +81980,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="91" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" ht="91" hidden="1" x14ac:dyDescent="0.35">
       <c r="A20" s="10" t="s">
         <v>854</v>
       </c>
@@ -81991,7 +81993,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="91" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" ht="91" hidden="1" x14ac:dyDescent="0.35">
       <c r="A21" s="10" t="s">
         <v>855</v>
       </c>
@@ -82004,7 +82006,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="91" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" ht="91" hidden="1" x14ac:dyDescent="0.35">
       <c r="A22" s="10" t="s">
         <v>239</v>
       </c>
@@ -82021,7 +82023,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="143" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" ht="143" hidden="1" x14ac:dyDescent="0.35">
       <c r="A23" s="10" t="s">
         <v>242</v>
       </c>
@@ -82034,7 +82036,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="65" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" ht="65" hidden="1" x14ac:dyDescent="0.35">
       <c r="A24" s="10" t="s">
         <v>236</v>
       </c>
@@ -82051,7 +82053,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="26" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" ht="26" hidden="1" x14ac:dyDescent="0.35">
       <c r="A25" s="10" t="s">
         <v>858</v>
       </c>
@@ -82085,7 +82087,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="390" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" ht="390" hidden="1" x14ac:dyDescent="0.35">
       <c r="A27" s="10" t="s">
         <v>866</v>
       </c>
@@ -82098,7 +82100,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="143" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" ht="143" hidden="1" x14ac:dyDescent="0.35">
       <c r="A28" s="10" t="s">
         <v>867</v>
       </c>
@@ -82111,7 +82113,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="208" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" ht="208" hidden="1" x14ac:dyDescent="0.35">
       <c r="A29" s="10" t="s">
         <v>868</v>
       </c>
@@ -82124,7 +82126,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="39" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" ht="39" hidden="1" x14ac:dyDescent="0.35">
       <c r="A30" s="10" t="s">
         <v>3337</v>
       </c>
@@ -82141,7 +82143,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="39" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" ht="39" hidden="1" x14ac:dyDescent="0.35">
       <c r="A31" s="10" t="s">
         <v>240</v>
       </c>
@@ -82156,7 +82158,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="39" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" ht="39" hidden="1" x14ac:dyDescent="0.35">
       <c r="A32" s="10" t="s">
         <v>243</v>
       </c>
@@ -82171,7 +82173,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="91" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" ht="91" hidden="1" x14ac:dyDescent="0.35">
       <c r="A33" s="10" t="s">
         <v>204</v>
       </c>
@@ -82188,7 +82190,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="169" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" ht="169" hidden="1" x14ac:dyDescent="0.35">
       <c r="A34" s="10" t="s">
         <v>241</v>
       </c>
@@ -82201,7 +82203,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="26" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" ht="26" hidden="1" x14ac:dyDescent="0.35">
       <c r="A35" s="10" t="s">
         <v>875</v>
       </c>
@@ -82218,7 +82220,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="91" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" ht="91" hidden="1" x14ac:dyDescent="0.35">
       <c r="A36" s="10" t="s">
         <v>879</v>
       </c>
@@ -82235,7 +82237,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="286" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" ht="286" hidden="1" x14ac:dyDescent="0.35">
       <c r="A37" s="10" t="s">
         <v>881</v>
       </c>
@@ -82248,7 +82250,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="78" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" ht="78" hidden="1" x14ac:dyDescent="0.35">
       <c r="A38" s="10" t="s">
         <v>2995</v>
       </c>
@@ -82265,7 +82267,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="65" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" ht="65" hidden="1" x14ac:dyDescent="0.35">
       <c r="A39" s="10" t="s">
         <v>2972</v>
       </c>
@@ -82282,7 +82284,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="104" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" ht="104" hidden="1" x14ac:dyDescent="0.35">
       <c r="A40" s="10" t="s">
         <v>883</v>
       </c>
@@ -82299,7 +82301,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="65" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" ht="65" hidden="1" x14ac:dyDescent="0.35">
       <c r="A41" s="10" t="s">
         <v>885</v>
       </c>
@@ -82312,7 +82314,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="325" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" ht="325" hidden="1" x14ac:dyDescent="0.35">
       <c r="A42" s="10" t="s">
         <v>886</v>
       </c>
@@ -82325,7 +82327,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="104" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:5" ht="104" hidden="1" x14ac:dyDescent="0.35">
       <c r="A43" s="10" t="s">
         <v>887</v>
       </c>
@@ -82338,7 +82340,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="39" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:5" ht="39" hidden="1" x14ac:dyDescent="0.35">
       <c r="A44" s="10" t="s">
         <v>888</v>
       </c>
@@ -82355,7 +82357,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="104" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" ht="104" hidden="1" x14ac:dyDescent="0.35">
       <c r="A45" s="10" t="s">
         <v>891</v>
       </c>
@@ -82368,7 +82370,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="143" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:5" ht="143" hidden="1" x14ac:dyDescent="0.35">
       <c r="A46" s="10" t="s">
         <v>58</v>
       </c>
@@ -82385,7 +82387,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="156" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:5" ht="156" hidden="1" x14ac:dyDescent="0.35">
       <c r="A47" s="10" t="s">
         <v>895</v>
       </c>
@@ -82402,7 +82404,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="156" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:5" ht="156" hidden="1" x14ac:dyDescent="0.35">
       <c r="A48" s="10" t="s">
         <v>897</v>
       </c>
@@ -82419,7 +82421,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="52" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:5" ht="52" hidden="1" x14ac:dyDescent="0.35">
       <c r="A49" s="10" t="s">
         <v>899</v>
       </c>
@@ -82436,7 +82438,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="130" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:5" ht="130" hidden="1" x14ac:dyDescent="0.35">
       <c r="A50" s="10" t="s">
         <v>206</v>
       </c>
@@ -82453,7 +82455,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="39" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:5" ht="39" hidden="1" x14ac:dyDescent="0.35">
       <c r="A51" s="10" t="s">
         <v>903</v>
       </c>
@@ -82470,7 +82472,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="65" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:5" ht="65" hidden="1" x14ac:dyDescent="0.35">
       <c r="A52" s="10" t="s">
         <v>906</v>
       </c>
@@ -82487,7 +82489,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="91" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:5" ht="91" hidden="1" x14ac:dyDescent="0.35">
       <c r="A53" s="10" t="s">
         <v>205</v>
       </c>
@@ -82504,9 +82506,9 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="169" x14ac:dyDescent="0.35">
-      <c r="A54" s="10" t="s">
-        <v>2632</v>
+    <row r="54" spans="1:5" ht="169" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="10">
+        <v>7</v>
       </c>
       <c r="B54" s="11" t="s">
         <v>2728</v>
@@ -82517,7 +82519,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="325" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:5" ht="325" hidden="1" x14ac:dyDescent="0.35">
       <c r="A55" s="10" t="s">
         <v>911</v>
       </c>
@@ -82530,7 +82532,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="56" spans="1:5" ht="78" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:5" ht="78" hidden="1" x14ac:dyDescent="0.35">
       <c r="A56" s="10" t="s">
         <v>912</v>
       </c>
@@ -82547,7 +82549,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="57" spans="1:5" ht="117" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:5" ht="117" hidden="1" x14ac:dyDescent="0.35">
       <c r="A57" s="10" t="s">
         <v>915</v>
       </c>
@@ -82564,7 +82566,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="58" spans="1:5" ht="221" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:5" ht="221" hidden="1" x14ac:dyDescent="0.35">
       <c r="A58" s="10" t="s">
         <v>916</v>
       </c>
@@ -82577,7 +82579,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="59" spans="1:5" ht="143" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:5" ht="143" hidden="1" x14ac:dyDescent="0.35">
       <c r="A59" s="10" t="s">
         <v>917</v>
       </c>
@@ -82594,7 +82596,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="60" spans="1:5" ht="247" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:5" ht="247" hidden="1" x14ac:dyDescent="0.35">
       <c r="A60" s="10" t="s">
         <v>919</v>
       </c>
@@ -82607,7 +82609,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="61" spans="1:5" ht="247" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:5" ht="247" hidden="1" x14ac:dyDescent="0.35">
       <c r="A61" s="10" t="s">
         <v>920</v>
       </c>
@@ -82637,7 +82639,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="26" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:5" ht="26" hidden="1" x14ac:dyDescent="0.35">
       <c r="A63" s="10" t="s">
         <v>924</v>
       </c>
@@ -82654,7 +82656,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="64" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:5" ht="409.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A64" s="10" t="s">
         <v>928</v>
       </c>
@@ -82667,7 +82669,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="65" spans="1:5" ht="377" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:5" ht="377" hidden="1" x14ac:dyDescent="0.35">
       <c r="A65" s="10" t="s">
         <v>929</v>
       </c>
@@ -82680,7 +82682,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:5" ht="39" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:5" ht="39" hidden="1" x14ac:dyDescent="0.35">
       <c r="A66" s="10" t="s">
         <v>930</v>
       </c>
@@ -82697,7 +82699,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="67" spans="1:5" ht="39" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:5" ht="39" hidden="1" x14ac:dyDescent="0.35">
       <c r="A67" s="10" t="s">
         <v>932</v>
       </c>
@@ -82714,7 +82716,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="68" spans="1:5" ht="169" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:5" ht="169" hidden="1" x14ac:dyDescent="0.35">
       <c r="A68" s="10" t="s">
         <v>935</v>
       </c>
@@ -82727,7 +82729,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="69" spans="1:5" ht="39" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:5" ht="39" hidden="1" x14ac:dyDescent="0.35">
       <c r="A69" s="10" t="s">
         <v>936</v>
       </c>
@@ -82744,7 +82746,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="70" spans="1:5" ht="364" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:5" ht="364" hidden="1" x14ac:dyDescent="0.35">
       <c r="A70" s="10" t="s">
         <v>939</v>
       </c>
@@ -82757,7 +82759,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="71" spans="1:5" ht="91" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:5" ht="91" hidden="1" x14ac:dyDescent="0.35">
       <c r="A71" s="10" t="s">
         <v>940</v>
       </c>
@@ -82774,7 +82776,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="72" spans="1:5" ht="143" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:5" ht="143" hidden="1" x14ac:dyDescent="0.35">
       <c r="A72" s="10" t="s">
         <v>942</v>
       </c>
@@ -82787,7 +82789,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="73" spans="1:5" ht="169" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:5" ht="169" hidden="1" x14ac:dyDescent="0.35">
       <c r="A73" s="10" t="s">
         <v>944</v>
       </c>
@@ -82813,7 +82815,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="75" spans="1:5" ht="78" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:5" ht="78" hidden="1" x14ac:dyDescent="0.35">
       <c r="A75" s="10" t="s">
         <v>947</v>
       </c>
@@ -82830,7 +82832,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="76" spans="1:5" ht="117" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:5" ht="117" hidden="1" x14ac:dyDescent="0.35">
       <c r="A76" s="10" t="s">
         <v>950</v>
       </c>
@@ -82843,7 +82845,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="77" spans="1:5" ht="39" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:5" ht="39" hidden="1" x14ac:dyDescent="0.35">
       <c r="A77" s="10" t="s">
         <v>951</v>
       </c>
@@ -82860,7 +82862,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="78" spans="1:5" ht="143" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:5" ht="143" hidden="1" x14ac:dyDescent="0.35">
       <c r="A78" s="10" t="s">
         <v>953</v>
       </c>
@@ -82873,7 +82875,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="79" spans="1:5" ht="65" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:5" ht="65" hidden="1" x14ac:dyDescent="0.35">
       <c r="A79" s="10" t="s">
         <v>954</v>
       </c>
@@ -82890,7 +82892,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="80" spans="1:5" ht="195" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:5" ht="195" hidden="1" x14ac:dyDescent="0.35">
       <c r="A80" s="10" t="s">
         <v>956</v>
       </c>
@@ -82903,7 +82905,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="81" spans="1:5" ht="299" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:5" ht="299" hidden="1" x14ac:dyDescent="0.35">
       <c r="A81" s="10" t="s">
         <v>957</v>
       </c>
@@ -82916,7 +82918,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="82" spans="1:5" ht="143" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:5" ht="143" hidden="1" x14ac:dyDescent="0.35">
       <c r="A82" s="25" t="s">
         <v>3608</v>
       </c>
@@ -82933,7 +82935,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="83" spans="1:5" ht="143" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:5" ht="143" hidden="1" x14ac:dyDescent="0.35">
       <c r="A83" s="25" t="s">
         <v>3617</v>
       </c>
@@ -82950,7 +82952,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="84" spans="1:5" ht="52" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:5" ht="52" hidden="1" x14ac:dyDescent="0.35">
       <c r="A84" s="25" t="s">
         <v>3618</v>
       </c>
@@ -82967,7 +82969,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="85" spans="1:5" ht="65" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:5" ht="65" hidden="1" x14ac:dyDescent="0.35">
       <c r="A85" s="25" t="s">
         <v>3399</v>
       </c>
@@ -82984,7 +82986,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="86" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:5" ht="58" hidden="1" x14ac:dyDescent="0.35">
       <c r="A86" s="25" t="s">
         <v>1448</v>
       </c>
@@ -83001,7 +83003,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="87" spans="1:5" ht="91" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:5" ht="91" hidden="1" x14ac:dyDescent="0.35">
       <c r="A87" s="25" t="s">
         <v>2910</v>
       </c>
@@ -83018,7 +83020,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="88" spans="1:5" s="1" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:5" s="1" customFormat="1" ht="58" hidden="1" x14ac:dyDescent="0.35">
       <c r="A88" s="25" t="s">
         <v>3643</v>
       </c>
@@ -83035,7 +83037,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A89" s="25" t="s">
         <v>3644</v>
       </c>
@@ -83053,6 +83055,13 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:E89" xr:uid="{46B3BDA4-C76D-4F2B-A5C7-6A022A2D593F}">
+    <filterColumn colId="4">
+      <filters>
+        <filter val="0.5"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -92198,7 +92207,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{041E0963-E2E9-41B5-B435-BC1A1C291BC2}">
   <dimension ref="A1:D91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+    <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
@@ -92841,7 +92850,7 @@
         <v>2667</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="65" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:4" ht="52" x14ac:dyDescent="0.35">
       <c r="A46" s="12" t="s">
         <v>2669</v>
       </c>

</xml_diff>

<commit_message>
Add leader to Game Mode
</commit_message>
<xml_diff>
--- a/src/data/mesbg_data.xlsx
+++ b/src/data/mesbg_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alex_\Downloads\mesbg-list-builder\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0AAB38E-8FC1-4F8F-AECF-2A7C2968441D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C646EB6D-41DE-4270-8985-0E81DAC1BB14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="1" xr2:uid="{41642CF3-1564-4507-B9B3-31F38315AF34}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="4" xr2:uid="{41642CF3-1564-4507-B9B3-31F38315AF34}"/>
   </bookViews>
   <sheets>
     <sheet name="models" sheetId="1" r:id="rId1"/>
@@ -24,6 +24,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">hero_constraints!$A$1:$E$511</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">models!$A$1:$L$895</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">options!$A$1:$G$1649</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">warning_rules!$A$1:$D$89</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -46474,7 +46475,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BD621D9-338F-4B24-B8C0-543A62D24772}">
   <dimension ref="A1:G1683"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A1663" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B1683" sqref="B1683"/>
     </sheetView>
@@ -93057,10 +93058,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{041E0963-E2E9-41B5-B435-BC1A1C291BC2}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:D89"/>
   <sheetViews>
-    <sheetView topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="A90" sqref="A90:XFD91"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="13" x14ac:dyDescent="0.35"/>
@@ -93086,7 +93088,7 @@
         <v>1534</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
         <v>1539</v>
       </c>
@@ -93100,7 +93102,7 @@
         <v>1540</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A3" s="12" t="s">
         <v>1100</v>
       </c>
@@ -93114,7 +93116,7 @@
         <v>1545</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="39" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" ht="39" hidden="1" x14ac:dyDescent="0.35">
       <c r="A4" s="12" t="s">
         <v>1293</v>
       </c>
@@ -93128,7 +93130,7 @@
         <v>1551</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A5" s="12" t="s">
         <v>1498</v>
       </c>
@@ -93184,7 +93186,7 @@
         <v>1558</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="65" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" ht="65" hidden="1" x14ac:dyDescent="0.35">
       <c r="A9" s="12" t="s">
         <v>1009</v>
       </c>
@@ -93198,7 +93200,7 @@
         <v>1559</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A10" s="12" t="s">
         <v>1013</v>
       </c>
@@ -93240,7 +93242,7 @@
         <v>3076</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="52" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" ht="52" hidden="1" x14ac:dyDescent="0.35">
       <c r="A13" s="12" t="s">
         <v>1075</v>
       </c>
@@ -93254,7 +93256,7 @@
         <v>3075</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A14" s="12" t="s">
         <v>1082</v>
       </c>
@@ -93296,7 +93298,7 @@
         <v>3846</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A17" s="12" t="s">
         <v>944</v>
       </c>
@@ -93310,7 +93312,7 @@
         <v>1593</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A18" s="12" t="s">
         <v>1594</v>
       </c>
@@ -93324,7 +93326,7 @@
         <v>1596</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A19" s="12" t="s">
         <v>1599</v>
       </c>
@@ -93338,7 +93340,7 @@
         <v>1598</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A20" s="12" t="s">
         <v>839</v>
       </c>
@@ -93352,7 +93354,7 @@
         <v>1632</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A21" s="12" t="s">
         <v>1636</v>
       </c>
@@ -93366,7 +93368,7 @@
         <v>1668</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A22" s="12" t="s">
         <v>942</v>
       </c>
@@ -93380,7 +93382,7 @@
         <v>1709</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A23" s="12" t="s">
         <v>868</v>
       </c>
@@ -93394,7 +93396,7 @@
         <v>1668</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A24" s="12" t="s">
         <v>867</v>
       </c>
@@ -93408,7 +93410,7 @@
         <v>1779</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A25" s="12" t="s">
         <v>840</v>
       </c>
@@ -93422,7 +93424,7 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A26" s="12" t="s">
         <v>881</v>
       </c>
@@ -93436,7 +93438,7 @@
         <v>1668</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A27" s="12" t="s">
         <v>881</v>
       </c>
@@ -93450,7 +93452,7 @@
         <v>1837</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A28" s="12" t="s">
         <v>881</v>
       </c>
@@ -93464,7 +93466,7 @@
         <v>1838</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A29" s="12" t="s">
         <v>891</v>
       </c>
@@ -93478,7 +93480,7 @@
         <v>1862</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A30" s="12" t="s">
         <v>866</v>
       </c>
@@ -93492,7 +93494,7 @@
         <v>1632</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A31" s="12" t="s">
         <v>957</v>
       </c>
@@ -93506,7 +93508,7 @@
         <v>2091</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A32" s="12" t="s">
         <v>957</v>
       </c>
@@ -93520,7 +93522,7 @@
         <v>2090</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A33" s="12" t="s">
         <v>854</v>
       </c>
@@ -93534,7 +93536,7 @@
         <v>2092</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="26" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" ht="26" hidden="1" x14ac:dyDescent="0.35">
       <c r="A34" s="12" t="s">
         <v>945</v>
       </c>
@@ -93548,7 +93550,7 @@
         <v>2154</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="39" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" ht="39" hidden="1" x14ac:dyDescent="0.35">
       <c r="A35" s="12" t="s">
         <v>945</v>
       </c>
@@ -93562,7 +93564,7 @@
         <v>2156</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A36" s="12" t="s">
         <v>855</v>
       </c>
@@ -93576,7 +93578,7 @@
         <v>2703</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A37" s="12" t="s">
         <v>849</v>
       </c>
@@ -93590,7 +93592,7 @@
         <v>2193</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A38" s="12" t="s">
         <v>916</v>
       </c>
@@ -93604,7 +93606,7 @@
         <v>2218</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A39" s="12" t="s">
         <v>911</v>
       </c>
@@ -93618,7 +93620,7 @@
         <v>2226</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A40" s="12" t="s">
         <v>919</v>
       </c>
@@ -93632,7 +93634,7 @@
         <v>2260</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A41" s="12" t="s">
         <v>919</v>
       </c>
@@ -93646,7 +93648,7 @@
         <v>2261</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A42" s="12" t="s">
         <v>850</v>
       </c>
@@ -93660,7 +93662,7 @@
         <v>2588</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A43" s="12" t="s">
         <v>851</v>
       </c>
@@ -93674,7 +93676,7 @@
         <v>2615</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A44" s="12" t="s">
         <v>2632</v>
       </c>
@@ -93688,7 +93690,7 @@
         <v>3744</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A45" s="12" t="s">
         <v>887</v>
       </c>
@@ -93702,7 +93704,7 @@
         <v>2667</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="52" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:4" ht="52" hidden="1" x14ac:dyDescent="0.35">
       <c r="A46" s="12" t="s">
         <v>2669</v>
       </c>
@@ -93716,7 +93718,7 @@
         <v>2689</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A47" s="12" t="s">
         <v>944</v>
       </c>
@@ -93730,7 +93732,7 @@
         <v>2708</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A48" s="12" t="s">
         <v>944</v>
       </c>
@@ -93744,7 +93746,7 @@
         <v>2709</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A49" s="12" t="s">
         <v>944</v>
       </c>
@@ -93758,7 +93760,7 @@
         <v>2710</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="26" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:4" ht="26" hidden="1" x14ac:dyDescent="0.35">
       <c r="A50" s="12" t="s">
         <v>2733</v>
       </c>
@@ -93772,7 +93774,7 @@
         <v>2734</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="52" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:4" ht="52" hidden="1" x14ac:dyDescent="0.35">
       <c r="A51" s="12" t="s">
         <v>2992</v>
       </c>
@@ -93786,7 +93788,7 @@
         <v>2971</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="26" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:4" ht="26" hidden="1" x14ac:dyDescent="0.35">
       <c r="A52" s="12" t="s">
         <v>3103</v>
       </c>
@@ -93800,7 +93802,7 @@
         <v>3136</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="26" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:4" ht="26" hidden="1" x14ac:dyDescent="0.35">
       <c r="A53" s="12" t="s">
         <v>3120</v>
       </c>
@@ -93814,7 +93816,7 @@
         <v>3137</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A54" s="12" t="s">
         <v>3260</v>
       </c>
@@ -93828,7 +93830,7 @@
         <v>3687</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A55" s="12" t="s">
         <v>3262</v>
       </c>
@@ -93842,7 +93844,7 @@
         <v>3688</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A56" s="12" t="s">
         <v>3263</v>
       </c>
@@ -93856,7 +93858,7 @@
         <v>3689</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A57" s="12" t="s">
         <v>3694</v>
       </c>
@@ -93870,7 +93872,7 @@
         <v>3690</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A58" s="12" t="s">
         <v>3269</v>
       </c>
@@ -93884,7 +93886,7 @@
         <v>3273</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A59" s="12" t="s">
         <v>3270</v>
       </c>
@@ -93898,7 +93900,7 @@
         <v>3274</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A60" s="12" t="s">
         <v>3271</v>
       </c>
@@ -93912,7 +93914,7 @@
         <v>3276</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A61" s="12" t="s">
         <v>3272</v>
       </c>
@@ -94024,7 +94026,7 @@
         <v>3283</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="26" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:4" ht="26" hidden="1" x14ac:dyDescent="0.35">
       <c r="A69" s="24" t="s">
         <v>3311</v>
       </c>
@@ -94038,7 +94040,7 @@
         <v>3313</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="26" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:4" ht="26" hidden="1" x14ac:dyDescent="0.35">
       <c r="A70" s="24" t="s">
         <v>3333</v>
       </c>
@@ -94052,7 +94054,7 @@
         <v>3336</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A71" s="6" t="s">
         <v>928</v>
       </c>
@@ -94066,7 +94068,7 @@
         <v>3389</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A72" s="6" t="s">
         <v>928</v>
       </c>
@@ -94080,7 +94082,7 @@
         <v>3398</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A73" s="6" t="s">
         <v>928</v>
       </c>
@@ -94094,7 +94096,7 @@
         <v>3397</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="26" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:4" ht="26" hidden="1" x14ac:dyDescent="0.35">
       <c r="A74" s="12" t="s">
         <v>929</v>
       </c>
@@ -94108,7 +94110,7 @@
         <v>3396</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A75" s="12" t="s">
         <v>885</v>
       </c>
@@ -94122,7 +94124,7 @@
         <v>3426</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="104" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:4" ht="104" hidden="1" x14ac:dyDescent="0.35">
       <c r="A76" s="12" t="s">
         <v>886</v>
       </c>
@@ -94136,7 +94138,7 @@
         <v>3496</v>
       </c>
     </row>
-    <row r="77" spans="1:4" ht="26" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:4" ht="26" hidden="1" x14ac:dyDescent="0.35">
       <c r="A77" s="12" t="s">
         <v>886</v>
       </c>
@@ -94150,7 +94152,7 @@
         <v>3495</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A78" s="12" t="s">
         <v>953</v>
       </c>
@@ -94164,7 +94166,7 @@
         <v>3494</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A79" s="12" t="s">
         <v>935</v>
       </c>
@@ -94178,7 +94180,7 @@
         <v>3514</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A80" s="12" t="s">
         <v>950</v>
       </c>
@@ -94192,7 +94194,7 @@
         <v>3549</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A81" s="12" t="s">
         <v>939</v>
       </c>
@@ -94206,7 +94208,7 @@
         <v>3597</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A82" s="12" t="s">
         <v>939</v>
       </c>
@@ -94220,7 +94222,7 @@
         <v>3598</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A83" s="12" t="s">
         <v>242</v>
       </c>
@@ -94234,7 +94236,7 @@
         <v>3601</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A84" s="12" t="s">
         <v>242</v>
       </c>
@@ -94248,7 +94250,7 @@
         <v>3602</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A85" s="6" t="s">
         <v>241</v>
       </c>
@@ -94262,7 +94264,7 @@
         <v>3606</v>
       </c>
     </row>
-    <row r="86" spans="1:4" ht="26" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:4" ht="26" hidden="1" x14ac:dyDescent="0.35">
       <c r="A86" s="12" t="s">
         <v>3643</v>
       </c>
@@ -94276,7 +94278,7 @@
         <v>3670</v>
       </c>
     </row>
-    <row r="87" spans="1:4" ht="26" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:4" ht="26" hidden="1" x14ac:dyDescent="0.35">
       <c r="A87" s="12" t="s">
         <v>3644</v>
       </c>
@@ -94290,7 +94292,7 @@
         <v>3695</v>
       </c>
     </row>
-    <row r="88" spans="1:4" ht="26" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:4" ht="26" hidden="1" x14ac:dyDescent="0.35">
       <c r="A88" s="12" t="s">
         <v>3399</v>
       </c>
@@ -94304,7 +94306,7 @@
         <v>3671</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A89" s="12" t="s">
         <v>2910</v>
       </c>
@@ -94319,6 +94321,23 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:D89" xr:uid="{041E0963-E2E9-41B5-B435-BC1A1C291BC2}">
+    <filterColumn colId="3">
+      <filters>
+        <filter val="(Dark Denizens of Mirkwood) Warrior models may not lead warbands if the alliance level is 'Convenient' or 'Impossible', due to losing the necessary army bonus."/>
+        <filter val="(Sharkey's Rogues) Warrior models may not lead warbands if the alliance level is 'Convenient' or 'Impossible', due to losing the necessary army bonus."/>
+        <filter val="(The Dead of Dunharrow) Warrior models may not lead warbands if the alliance level is 'Convenient' or 'Impossible', due to losing the necessary army bonus."/>
+        <filter val="(Wildmen of Druadan) Warrior models may not lead warbands if the alliance level is 'Convenient' or 'Impossible', due to losing the necessary army bonus."/>
+        <filter val="If Arathorn is included in the same force as Aragorn, you automatically lose your army bonus and become impossible allies with all other army lists."/>
+        <filter val="If Bandobras Took is included in the same force as any named Hobbit Hero models, you automatically lose your army bonus and become impossible allies with all other army lists."/>
+        <filter val="If Bilbo is included in the same force as Frodo, Sam, Merry or Pippin, you automatically lose your army bonus and become impossible allies with all other army lists."/>
+        <filter val="If Eorl the Young is included in the same force as any named Rohan Hero models, you automatically lose your army bonus and become impossible allies with all other army lists."/>
+        <filter val="If Gil-Galad is included in the same force as either Arwen, Lindir, Elladan &amp; Elrohir or Bilbo Baggins, you automatically become Impossible Allies with all armies, and lose your army bonus."/>
+        <filter val="If Gil-Galad is included in the your force, you automatically become Impossible Allies with all except Numenor (Historical) and Lothlorien, Fangorn and The Misty Mountains (Convenient)."/>
+        <filter val="If Helm Hammerhand is included in your force, you automatically become impossible allies with all other army lists."/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>